<commit_message>
Added module 2 exercise
</commit_message>
<xml_diff>
--- a/Module 2/1- Unicorn Name/Unicorn Name.xlsx
+++ b/Module 2/1- Unicorn Name/Unicorn Name.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianca.dragu\Documents\UiPath\Unicorn Name\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmun\Desktop\SCS-3757-Robotic-and-Intelligent-Process-Automation\Module 2\1- Unicorn Name\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{422F5C19-87A6-4DE9-A2CF-DDC371667C27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{EDF95EE4-9E56-45FD-8DAB-87F998151032}"/>
+    <workbookView minimized="1" xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -44,16 +43,19 @@
     <t>Birthday Month</t>
   </si>
   <si>
-    <t>Alex</t>
-  </si>
-  <si>
-    <t>June</t>
+    <t>Edmund</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>Brave Crystal-Dazzler</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -413,21 +415,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{091E917C-F64A-40F0-9399-66F2A61F8C21}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.21875" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
-    <col min="3" max="3" width="30.21875" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,12 +440,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>